<commit_message>
set pass and set user name
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\תכנות\year 2\בדיקות ואיכות\final\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF315140-B9EE-4DA9-A76D-054E9EEEE691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54E28B-AE35-4F39-9427-2E07062F63FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{CB2C1D9B-843A-4C3B-B57D-582EAB370EF6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>girl</t>
+  </si>
+  <si>
+    <t>balance</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C044269E-8E80-4700-AB14-691E1B5F57AC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -450,7 +453,7 @@
     <col min="5" max="5" width="13.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +469,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -482,6 +488,9 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding sapir's code, and modify the register to set the passChar as **
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\תכנות\year 2\בדיקות ואיכות\final\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B54E28B-AE35-4F39-9427-2E07062F63FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685D7088-56BF-4666-A7E5-4C5818784653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8928" xr2:uid="{CB2C1D9B-843A-4C3B-B57D-582EAB370EF6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>balance</t>
+  </si>
+  <si>
+    <t>moshe1</t>
+  </si>
+  <si>
+    <t>Mm1122334!</t>
+  </si>
+  <si>
+    <t>moses@gmail.com</t>
+  </si>
+  <si>
+    <t>boy</t>
   </si>
 </sst>
 </file>
@@ -438,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C044269E-8E80-4700-AB14-691E1B5F57AC}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -493,6 +505,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>206676850</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added menu form - need to fix in-games problems
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -623,7 +623,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1009</x:v>
+        <x:v>1000</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -803,6 +803,726 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F15" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F16" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F17" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F18" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F19" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F20" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F21" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F22" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F23" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F24" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F25" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F26" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F27" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F28" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F29" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F30" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F31" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F32" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F33" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F34" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F35" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F36" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F37" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F38" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F39" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F40" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F41" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F42" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F43" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F44" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F45" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="A46" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F46" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="A47" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F47" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6">
+      <x:c r="A48" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F48" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6">
+      <x:c r="A49" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F49" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6">
+      <x:c r="A50" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F50" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="A51" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F51" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
fixed udi's in-game user data display
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1526,6 +1526,86 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="52" spans="1:6">
+      <x:c r="A52" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B52" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C52" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D52" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E52" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F52" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:6">
+      <x:c r="A53" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B53" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C53" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D53" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E53" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F53" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:6">
+      <x:c r="A54" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B54" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C54" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D54" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E54" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F54" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:6">
+      <x:c r="A55" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B55" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C55" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D55" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E55" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F55" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed udi's display and score logic
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -623,7 +623,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1000</x:v>
+        <x:v>1002</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -1603,6 +1603,86 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F55" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:6">
+      <x:c r="A56" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B56" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C56" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D56" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E56" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F56" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:6">
+      <x:c r="A57" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B57" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C57" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D57" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E57" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F57" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="58" spans="1:6">
+      <x:c r="A58" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B58" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C58" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D58" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E58" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F58" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="59" spans="1:6">
+      <x:c r="A59" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B59" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C59" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D59" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E59" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F59" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
fixed login, added get user func
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97254\source\repos\testing_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adf4de8bd431df76/Desktop/Software-Engineering/Year-B/Testing and Quality/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5530BFA3-E16D-4994-B9BA-4422C2D6C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5530BFA3-E16D-4994-B9BA-4422C2D6C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A74226-0FA9-4ECB-B120-C7DCFBB2F3DD}"/>
   <x:bookViews>
-    <x:workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7270" firstSheet="0" activeTab="0" xr2:uid="{CB2C1D9B-843A-4C3B-B57D-582EAB370EF6}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{CB2C1D9B-843A-4C3B-B57D-582EAB370EF6}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -108,6 +108,12 @@
   <x:si>
     <x:t>m@g.c</x:t>
   </x:si>
+  <x:si>
+    <x:t>udi</x:t>
+  </x:si>
+  <x:si>
+    <x:t>udi@udi</x:t>
+  </x:si>
 </x:sst>
 </file>
 
@@ -116,10 +122,19 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
+  <x:fonts count="3" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
+      <x:name val="Aptos Narrow"/>
+      <x:family val="2"/>
+      <x:charset val="177"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color theme="10"/>
       <x:name val="Aptos Narrow"/>
       <x:family val="2"/>
       <x:charset val="177"/>
@@ -150,13 +165,19 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </x:cellXfs>
-  <x:cellStyles count="1">
+  <x:cellStyles count="2">
+    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -491,22 +512,22 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F5"/>
+  <x:dimension ref="A1:F67"/>
   <x:sheetViews>
-    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <x:selection activeCell="D7" sqref="D7"/>
+    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <x:selection activeCell="F67" sqref="F67"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14"/>
+  <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.332031" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="15.375" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="20.75" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="18" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="27.25" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.25" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:6">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -526,7 +547,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:6">
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -546,7 +567,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:6">
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A3" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -566,7 +587,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:6">
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A4" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -586,7 +607,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:6">
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
@@ -606,7 +627,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:6">
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A6" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -623,10 +644,10 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1002</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:6">
+        <x:v>1000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A7" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -646,7 +667,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:6">
+    <x:row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A8" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -666,7 +687,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:6">
+    <x:row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A9" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -686,7 +707,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:6">
+    <x:row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A10" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -706,7 +727,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:6">
+    <x:row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A11" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -726,7 +747,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:6">
+    <x:row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A12" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -746,7 +767,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:6">
+    <x:row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A13" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -766,7 +787,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:6">
+    <x:row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A14" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -786,7 +807,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:6">
+    <x:row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A15" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -806,7 +827,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:6">
+    <x:row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A16" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -826,7 +847,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:6">
+    <x:row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A17" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -846,7 +867,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:6">
+    <x:row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A18" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -866,7 +887,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:6">
+    <x:row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A19" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -886,7 +907,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:6">
+    <x:row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A20" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -906,7 +927,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:6">
+    <x:row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A21" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -926,7 +947,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:6">
+    <x:row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A22" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -946,7 +967,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:6">
+    <x:row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A23" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -966,7 +987,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:6">
+    <x:row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A24" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -986,7 +1007,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="25" spans="1:6">
+    <x:row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A25" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1006,7 +1027,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="26" spans="1:6">
+    <x:row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A26" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1026,7 +1047,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="27" spans="1:6">
+    <x:row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A27" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1046,7 +1067,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:6">
+    <x:row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A28" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1066,7 +1087,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="29" spans="1:6">
+    <x:row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A29" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1086,7 +1107,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="30" spans="1:6">
+    <x:row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A30" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1106,7 +1127,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="31" spans="1:6">
+    <x:row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A31" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1126,7 +1147,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="32" spans="1:6">
+    <x:row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A32" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1146,7 +1167,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="33" spans="1:6">
+    <x:row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A33" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1166,7 +1187,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="34" spans="1:6">
+    <x:row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A34" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1186,7 +1207,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="35" spans="1:6">
+    <x:row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A35" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1206,7 +1227,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="36" spans="1:6">
+    <x:row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A36" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1226,7 +1247,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="37" spans="1:6">
+    <x:row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A37" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1246,7 +1267,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="38" spans="1:6">
+    <x:row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A38" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1266,7 +1287,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="39" spans="1:6">
+    <x:row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A39" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1286,7 +1307,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="40" spans="1:6">
+    <x:row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A40" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1306,7 +1327,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="41" spans="1:6">
+    <x:row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A41" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1326,7 +1347,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="42" spans="1:6">
+    <x:row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A42" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1346,7 +1367,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="43" spans="1:6">
+    <x:row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A43" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1366,7 +1387,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="44" spans="1:6">
+    <x:row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A44" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1386,7 +1407,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="45" spans="1:6">
+    <x:row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A45" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1406,7 +1427,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="46" spans="1:6">
+    <x:row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A46" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1426,7 +1447,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="47" spans="1:6">
+    <x:row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A47" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1446,7 +1467,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="48" spans="1:6">
+    <x:row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A48" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1466,7 +1487,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="49" spans="1:6">
+    <x:row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A49" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1486,7 +1507,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="50" spans="1:6">
+    <x:row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A50" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1506,7 +1527,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="51" spans="1:6">
+    <x:row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A51" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1526,7 +1547,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="52" spans="1:6">
+    <x:row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A52" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1546,7 +1567,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="53" spans="1:6">
+    <x:row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A53" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1566,7 +1587,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="54" spans="1:6">
+    <x:row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A54" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1586,7 +1607,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="55" spans="1:6">
+    <x:row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A55" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1606,7 +1627,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="56" spans="1:6">
+    <x:row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A56" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1626,7 +1647,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="57" spans="1:6">
+    <x:row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A57" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1646,7 +1667,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="58" spans="1:6">
+    <x:row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A58" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1666,7 +1687,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="59" spans="1:6">
+    <x:row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A59" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1686,7 +1707,190 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A60" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B60" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C60" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D60" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E60" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F60" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A61" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B61" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C61" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D61" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E61" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F61" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A62" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B62" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C62" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D62" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E62" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F62" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A63" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B63" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C63" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D63" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E63" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F63" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A64" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B64" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C64" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D64" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E64" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F64" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A65" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B65" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C65" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D65" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E65" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F65" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A66" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B66" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C66" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D66" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E66" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F66" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A67" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B67" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C67" s="0">
+        <x:v>1234</x:v>
+      </x:c>
+      <x:c r="D67" s="1" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="E67" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F67" s="0">
+        <x:v>100</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="68" spans="1:6">
+      <x:c r="A68" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B68" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C68" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D68" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E68" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F68" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="D67" r:id="rId6"/>
+  </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
adding close button ti user interface
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1887,6 +1887,166 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="69" spans="1:6">
+      <x:c r="A69" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B69" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C69" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D69" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E69" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F69" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:6">
+      <x:c r="A70" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B70" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C70" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D70" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E70" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F70" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="71" spans="1:6">
+      <x:c r="A71" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B71" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C71" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D71" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E71" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F71" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="72" spans="1:6">
+      <x:c r="A72" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B72" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C72" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D72" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E72" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F72" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="73" spans="1:6">
+      <x:c r="A73" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B73" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C73" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D73" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E73" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F73" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="74" spans="1:6">
+      <x:c r="A74" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B74" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C74" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D74" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E74" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F74" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="75" spans="1:6">
+      <x:c r="A75" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B75" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C75" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D75" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E75" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F75" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="76" spans="1:6">
+      <x:c r="A76" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B76" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C76" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D76" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E76" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F76" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId6"/>

</xml_diff>

<commit_message>
FULL DESIGN OF THE PROJECT+added timer my game+user info in my game
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -32,83 +32,6 @@
     </x:ext>
   </x:extLst>
 </x:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:si>
-    <x:t>Username</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Password</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ID</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Email</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Gender</x:t>
-  </x:si>
-  <x:si>
-    <x:t>balance</x:t>
-  </x:si>
-  <x:si>
-    <x:t>liora18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>liora18!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>liora@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>girl</x:t>
-  </x:si>
-  <x:si>
-    <x:t>moshe1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Mm1122334!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>moses@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>boy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hliran2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hliran2@</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hliran2@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Male</x:t>
-  </x:si>
-  <x:si>
-    <x:t>liran12</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hliran2@</x:t>
-  </x:si>
-  <x:si>
-    <x:t>moses</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bro</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m@g.c</x:t>
-  </x:si>
-</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -623,7 +546,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1009</x:v>
+        <x:v>1000</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6">
@@ -803,6 +726,726 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F15" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:6">
+      <x:c r="A16" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F16" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:6">
+      <x:c r="A17" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F17" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:6">
+      <x:c r="A18" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F18" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D19" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F19" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:6">
+      <x:c r="A20" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D20" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F20" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:6">
+      <x:c r="A21" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E21" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F21" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:6">
+      <x:c r="A22" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E22" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F22" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:6">
+      <x:c r="A23" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E23" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F23" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:6">
+      <x:c r="A24" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E24" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F24" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:6">
+      <x:c r="A25" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C25" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D25" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E25" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F25" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:6">
+      <x:c r="A26" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E26" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F26" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:6">
+      <x:c r="A27" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E27" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F27" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:6">
+      <x:c r="A28" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F28" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:6">
+      <x:c r="A29" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E29" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F29" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:6">
+      <x:c r="A30" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E30" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F30" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:6">
+      <x:c r="A31" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E31" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F31" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:6">
+      <x:c r="A32" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E32" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F32" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:6">
+      <x:c r="A33" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E33" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F33" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E34" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F34" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B35" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C35" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D35" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E35" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F35" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B36" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C36" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D36" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E36" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F36" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B37" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C37" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D37" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E37" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F37" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B38" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C38" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D38" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E38" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F38" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B39" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C39" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D39" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E39" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F39" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B40" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C40" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D40" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E40" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F40" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B41" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C41" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D41" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E41" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F41" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B42" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C42" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D42" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E42" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F42" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B43" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C43" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D43" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E43" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F43" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B44" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C44" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D44" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E44" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F44" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B45" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C45" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D45" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E45" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F45" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:6">
+      <x:c r="A46" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B46" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C46" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D46" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E46" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F46" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:6">
+      <x:c r="A47" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B47" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C47" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D47" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E47" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F47" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:6">
+      <x:c r="A48" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B48" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C48" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D48" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E48" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F48" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:6">
+      <x:c r="A49" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B49" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C49" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D49" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E49" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F49" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:6">
+      <x:c r="A50" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B50" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C50" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D50" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E50" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F50" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:6">
+      <x:c r="A51" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B51" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C51" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D51" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E51" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F51" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
updated login and register
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -2334,6 +2334,46 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="90" spans="1:6">
+      <x:c r="A90" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F90" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:6">
+      <x:c r="A91" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId7"/>

</xml_diff>

<commit_message>
needs to fix SetBalance method in DB
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -5,7 +5,7 @@
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adf4de8bd431df76/Desktop/Software-Engineering/Year-B/Testing and Quality/git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adf4de8bd431df76/Desktop/Software-Engineering/Year-B/Testing and Quality/git2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5530BFA3-E16D-4994-B9BA-4422C2D6C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A74226-0FA9-4ECB-B120-C7DCFBB2F3DD}"/>
@@ -539,9 +539,9 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F67"/>
+  <x:dimension ref="A1:F91"/>
   <x:sheetViews>
-    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <x:selection activeCell="F67" sqref="F67"/>
     </x:sheetView>
   </x:sheetViews>
@@ -671,7 +671,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1000</x:v>
+        <x:v>1008</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1894,7 +1894,7 @@
         <x:v>100</x:v>
       </x:c>
     </x:row>
-    <x:row r="68" spans="1:6">
+    <x:row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A68" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1914,7 +1914,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="69" spans="1:6">
+    <x:row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A69" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1934,7 +1934,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="70" spans="1:6">
+    <x:row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A70" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1954,7 +1954,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="71" spans="1:6">
+    <x:row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A71" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1974,7 +1974,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="72" spans="1:6">
+    <x:row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A72" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1994,7 +1994,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="73" spans="1:6">
+    <x:row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A73" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2014,7 +2014,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="74" spans="1:6">
+    <x:row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A74" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2034,7 +2034,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="75" spans="1:6">
+    <x:row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A75" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2054,7 +2054,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="76" spans="1:6">
+    <x:row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A76" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2074,7 +2074,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="77" spans="1:6">
+    <x:row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A77" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2094,7 +2094,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="78" spans="1:6">
+    <x:row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A78" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2114,7 +2114,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="79" spans="1:6">
+    <x:row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A79" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2134,7 +2134,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="80" spans="1:6">
+    <x:row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A80" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2154,7 +2154,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="81" spans="1:6">
+    <x:row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A81" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2174,7 +2174,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="82" spans="1:6">
+    <x:row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A82" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2194,7 +2194,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="83" spans="1:6">
+    <x:row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A83" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2214,7 +2214,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="84" spans="1:6">
+    <x:row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A84" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2234,7 +2234,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="85" spans="1:6">
+    <x:row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A85" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2254,7 +2254,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="86" spans="1:6">
+    <x:row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A86" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
@@ -2274,7 +2274,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="87" spans="1:6">
+    <x:row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A87" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2294,7 +2294,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="88" spans="1:6">
+    <x:row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A88" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
@@ -2314,7 +2314,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="89" spans="1:6">
+    <x:row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A89" s="0" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -2331,6 +2331,66 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F89" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A90" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F90" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A91" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:6">
+      <x:c r="A92" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F92" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Fix the picture loading for the game and add background and fix the design
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -2374,9 +2374,129 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="92" spans="1:6">
+      <x:c r="A92" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F92" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:6">
+      <x:c r="A93" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:6">
+      <x:c r="A94" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F94" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:6">
+      <x:c r="A95" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:6">
+      <x:c r="A96" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E96" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F96" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:6">
+      <x:c r="A97" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added background to login form
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -671,7 +671,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1008</x:v>
+        <x:v>1000</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2391,6 +2391,166 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F92" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:6">
+      <x:c r="A93" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:6">
+      <x:c r="A94" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F94" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:6">
+      <x:c r="A95" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:6">
+      <x:c r="A96" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E96" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F96" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:6">
+      <x:c r="A97" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:6">
+      <x:c r="A98" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E98" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F98" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:6">
+      <x:c r="A99" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E99" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F99" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:6">
+      <x:c r="A100" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E100" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F100" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
fixed english memory game
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -644,7 +644,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1000</x:v>
+        <x:v>1032</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2047,9 +2047,749 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="77" spans="1:6">
+      <x:c r="A77" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B77" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C77" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D77" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E77" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F77" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="78" spans="1:6">
+      <x:c r="A78" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B78" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C78" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D78" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E78" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F78" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="79" spans="1:6">
+      <x:c r="A79" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B79" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C79" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D79" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E79" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F79" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="80" spans="1:6">
+      <x:c r="A80" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B80" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C80" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D80" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E80" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F80" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="81" spans="1:6">
+      <x:c r="A81" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B81" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C81" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D81" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E81" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F81" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:6">
+      <x:c r="A82" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B82" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C82" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D82" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E82" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F82" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="83" spans="1:6">
+      <x:c r="A83" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B83" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C83" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D83" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E83" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F83" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="84" spans="1:6">
+      <x:c r="A84" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B84" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C84" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D84" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E84" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F84" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="85" spans="1:6">
+      <x:c r="A85" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B85" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C85" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D85" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E85" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F85" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="86" spans="1:6">
+      <x:c r="A86" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B86" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C86" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D86" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E86" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F86" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:6">
+      <x:c r="A87" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B87" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C87" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D87" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E87" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F87" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="88" spans="1:6">
+      <x:c r="A88" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B88" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C88" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D88" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E88" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F88" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="89" spans="1:6">
+      <x:c r="A89" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B89" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C89" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D89" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E89" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F89" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="90" spans="1:6">
+      <x:c r="A90" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B90" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C90" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D90" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E90" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F90" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:6">
+      <x:c r="A91" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B91" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C91" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D91" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E91" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F91" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:6">
+      <x:c r="A92" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B92" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C92" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D92" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E92" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F92" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:6">
+      <x:c r="A93" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B93" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C93" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D93" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E93" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F93" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="94" spans="1:6">
+      <x:c r="A94" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B94" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C94" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D94" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E94" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F94" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="95" spans="1:6">
+      <x:c r="A95" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B95" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C95" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D95" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E95" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F95" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:6">
+      <x:c r="A96" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B96" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C96" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D96" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E96" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F96" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="97" spans="1:6">
+      <x:c r="A97" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B97" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C97" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D97" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E97" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F97" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="98" spans="1:6">
+      <x:c r="A98" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B98" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C98" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D98" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E98" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F98" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="99" spans="1:6">
+      <x:c r="A99" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B99" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C99" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D99" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E99" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F99" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="100" spans="1:6">
+      <x:c r="A100" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B100" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C100" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D100" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E100" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F100" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="101" spans="1:6">
+      <x:c r="A101" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B101" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C101" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D101" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E101" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F101" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:6">
+      <x:c r="A102" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B102" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C102" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D102" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E102" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F102" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:6">
+      <x:c r="A103" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C103" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E103" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F103" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:6">
+      <x:c r="A104" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C104" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D104" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E104" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F104" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:6">
+      <x:c r="A105" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D105" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E105" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F105" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:6">
+      <x:c r="A106" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C106" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D106" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E106" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F106" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:6">
+      <x:c r="A107" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C107" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E107" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:6">
+      <x:c r="A108" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C108" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D108" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E108" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F108" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:6">
+      <x:c r="A109" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C109" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E109" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:6">
+      <x:c r="A110" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C110" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D110" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E110" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F110" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:6">
+      <x:c r="A111" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E111" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:6">
+      <x:c r="A112" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C112" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D112" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E112" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F112" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:6">
+      <x:c r="A113" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C113" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D113" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E113" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F113" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId6"/>
+    <x:hyperlink ref="D67" r:id="rId7"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tried new udi's math game background
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -2594,9 +2594,89 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="103" spans="1:6">
+      <x:c r="A103" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B103" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C103" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D103" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E103" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F103" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:6">
+      <x:c r="A104" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B104" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C104" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D104" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E104" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F104" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="105" spans="1:6">
+      <x:c r="A105" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B105" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C105" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D105" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E105" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F105" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="106" spans="1:6">
+      <x:c r="A106" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B106" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C106" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D106" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E106" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F106" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated udi's game background
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -2674,6 +2674,166 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="107" spans="1:6">
+      <x:c r="A107" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B107" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C107" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D107" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E107" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F107" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="108" spans="1:6">
+      <x:c r="A108" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B108" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C108" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D108" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E108" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F108" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="109" spans="1:6">
+      <x:c r="A109" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B109" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C109" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D109" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E109" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F109" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="110" spans="1:6">
+      <x:c r="A110" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B110" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C110" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D110" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E110" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F110" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:6">
+      <x:c r="A111" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B111" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C111" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D111" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E111" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F111" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="112" spans="1:6">
+      <x:c r="A112" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B112" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C112" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D112" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E112" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F112" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="113" spans="1:6">
+      <x:c r="A113" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B113" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C113" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D113" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E113" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F113" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="114" spans="1:6">
+      <x:c r="A114" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B114" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C114" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D114" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E114" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F114" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId6"/>

</xml_diff>

<commit_message>
udi's game - updated graphics
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -2834,6 +2834,146 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="115" spans="1:6">
+      <x:c r="A115" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B115" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C115" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D115" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E115" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F115" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116" spans="1:6">
+      <x:c r="A116" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B116" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C116" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D116" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E116" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F116" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="117" spans="1:6">
+      <x:c r="A117" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B117" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C117" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D117" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E117" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F117" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="118" spans="1:6">
+      <x:c r="A118" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B118" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C118" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D118" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E118" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F118" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="119" spans="1:6">
+      <x:c r="A119" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B119" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C119" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D119" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E119" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F119" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="120" spans="1:6">
+      <x:c r="A120" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B120" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C120" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D120" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E120" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F120" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="121" spans="1:6">
+      <x:c r="A121" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B121" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C121" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D121" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E121" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F121" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId6"/>

</xml_diff>

<commit_message>
updated register password validation
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -3054,6 +3054,26 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="126" spans="1:6">
+      <x:c r="A126" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B126" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C126" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D126" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E126" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F126" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId6"/>

</xml_diff>

<commit_message>
merged with current master
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -671,7 +671,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>10010</x:v>
+        <x:v>120</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3294,9 +3294,69 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="138" spans="1:6">
+      <x:c r="A138" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B138" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C138" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D138" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E138" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F138" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="139" spans="1:6">
+      <x:c r="A139" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B139" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C139" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D139" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E139" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F139" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="140" spans="1:6">
+      <x:c r="A140" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B140" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C140" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D140" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E140" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F140" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tried to update store's design
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -648,7 +648,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>1000</x:v>
+        <x:v>520</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -668,12 +668,12 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F7" s="0">
-        <x:v>98295</x:v>
+        <x:v>98260</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D7" r:id="rId7"/>
+    <x:hyperlink ref="D7" r:id="rId8"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
only design windows and buttons
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -140,6 +140,18 @@
   </x:si>
   <x:si>
     <x:t>lira@jj.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dianka</x:t>
+  </x:si>
+  <x:si>
+    <x:t>D12345!1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123456789</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Diana@hey.com</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -3614,6 +3626,246 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="154" spans="1:6">
+      <x:c r="A154" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B154" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C154" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D154" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E154" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F154" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="155" spans="1:6">
+      <x:c r="A155" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B155" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C155" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D155" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E155" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F155" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="156" spans="1:6">
+      <x:c r="A156" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B156" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C156" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D156" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E156" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F156" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="157" spans="1:6">
+      <x:c r="A157" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B157" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C157" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D157" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E157" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F157" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="158" spans="1:6">
+      <x:c r="A158" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B158" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C158" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D158" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E158" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F158" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="159" spans="1:6">
+      <x:c r="A159" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B159" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C159" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D159" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E159" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F159" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="160" spans="1:6">
+      <x:c r="A160" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B160" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C160" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D160" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E160" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F160" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="161" spans="1:6">
+      <x:c r="A161" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B161" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C161" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D161" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E161" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F161" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="162" spans="1:6">
+      <x:c r="A162" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B162" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C162" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D162" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E162" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F162" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="163" spans="1:6">
+      <x:c r="A163" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B163" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C163" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D163" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E163" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F163" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="164" spans="1:6">
+      <x:c r="A164" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B164" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C164" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D164" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E164" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F164" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="165" spans="1:6">
+      <x:c r="A165" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B165" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C165" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D165" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E165" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="F165" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:hyperlinks>
     <x:hyperlink ref="D67" r:id="rId7"/>

</xml_diff>

<commit_message>
fixed look and feel, updated user balance from db in all forms
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adf4de8bd431df76/Desktop/Software-Engineering/Year-B/Testing and Quality/git2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/adf4de8bd431df76/Desktop/Software-Engineering/Year-B/Testing and Quality/git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{5530BFA3-E16D-4994-B9BA-4422C2D6C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A74226-0FA9-4ECB-B120-C7DCFBB2F3DD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{5530BFA3-E16D-4994-B9BA-4422C2D6C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9833D114-EE10-414E-B169-094C1248576A}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{CB2C1D9B-843A-4C3B-B57D-582EAB370EF6}"/>
   </x:bookViews>
@@ -152,6 +152,18 @@
   </x:si>
   <x:si>
     <x:t>Diana@hey.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>admin1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>admin123!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123123123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>admin@admin.com</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -551,10 +563,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:F91"/>
+  <x:dimension ref="A1:F166"/>
   <x:sheetViews>
-    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <x:selection activeCell="F67" sqref="F67"/>
+    <x:sheetView rightToLeft="1" tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <x:selection activeCell="F166" sqref="F166"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -683,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>165</x:v>
+        <x:v>187</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2386,7 +2398,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="92" spans="1:6">
+    <x:row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A92" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2406,7 +2418,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="93" spans="1:6">
+    <x:row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A93" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2426,7 +2438,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="94" spans="1:6">
+    <x:row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A94" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2446,7 +2458,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="95" spans="1:6">
+    <x:row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A95" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2466,7 +2478,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="96" spans="1:6">
+    <x:row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A96" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2486,7 +2498,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="97" spans="1:6">
+    <x:row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A97" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2506,7 +2518,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="98" spans="1:6">
+    <x:row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A98" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2526,7 +2538,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="99" spans="1:6">
+    <x:row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A99" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2546,7 +2558,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="100" spans="1:6">
+    <x:row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A100" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2566,7 +2578,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="101" spans="1:6">
+    <x:row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A101" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2586,7 +2598,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="102" spans="1:6">
+    <x:row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A102" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2606,7 +2618,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="103" spans="1:6">
+    <x:row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A103" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2626,7 +2638,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="104" spans="1:6">
+    <x:row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A104" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2646,7 +2658,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="105" spans="1:6">
+    <x:row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A105" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2666,7 +2678,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="106" spans="1:6">
+    <x:row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A106" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2686,7 +2698,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="107" spans="1:6">
+    <x:row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A107" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2706,7 +2718,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="108" spans="1:6">
+    <x:row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A108" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2726,7 +2738,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="109" spans="1:6">
+    <x:row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A109" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2746,7 +2758,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="110" spans="1:6">
+    <x:row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A110" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2766,7 +2778,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="111" spans="1:6">
+    <x:row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A111" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2786,7 +2798,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="112" spans="1:6">
+    <x:row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A112" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2806,7 +2818,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="113" spans="1:6">
+    <x:row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A113" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2826,7 +2838,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="114" spans="1:6">
+    <x:row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A114" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2846,7 +2858,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="115" spans="1:6">
+    <x:row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A115" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2866,7 +2878,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="116" spans="1:6">
+    <x:row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A116" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2886,7 +2898,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="117" spans="1:6">
+    <x:row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A117" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2906,7 +2918,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="118" spans="1:6">
+    <x:row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A118" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2926,7 +2938,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="119" spans="1:6">
+    <x:row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A119" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2946,7 +2958,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="120" spans="1:6">
+    <x:row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A120" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2966,7 +2978,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="121" spans="1:6">
+    <x:row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A121" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -2986,7 +2998,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="122" spans="1:6">
+    <x:row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A122" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3006,7 +3018,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="123" spans="1:6">
+    <x:row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A123" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3026,7 +3038,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="124" spans="1:6">
+    <x:row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A124" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3046,7 +3058,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="125" spans="1:6">
+    <x:row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A125" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3066,7 +3078,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="126" spans="1:6">
+    <x:row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A126" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3086,7 +3098,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="127" spans="1:6">
+    <x:row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A127" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3106,7 +3118,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="128" spans="1:6">
+    <x:row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A128" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3126,7 +3138,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="129" spans="1:6">
+    <x:row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A129" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3146,7 +3158,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="130" spans="1:6">
+    <x:row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A130" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3166,7 +3178,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="131" spans="1:6">
+    <x:row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A131" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3186,7 +3198,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="132" spans="1:6">
+    <x:row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A132" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3206,7 +3218,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="133" spans="1:6">
+    <x:row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A133" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3226,7 +3238,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="134" spans="1:6">
+    <x:row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A134" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3246,7 +3258,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="135" spans="1:6">
+    <x:row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A135" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3266,7 +3278,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="136" spans="1:6">
+    <x:row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A136" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3286,7 +3298,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="137" spans="1:6">
+    <x:row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A137" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3306,7 +3318,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="138" spans="1:6">
+    <x:row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A138" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3326,7 +3338,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="139" spans="1:6">
+    <x:row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A139" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3346,7 +3358,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="140" spans="1:6">
+    <x:row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A140" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3366,7 +3378,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="141" spans="1:6">
+    <x:row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A141" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3386,7 +3398,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="142" spans="1:6">
+    <x:row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A142" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3406,7 +3418,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="143" spans="1:6">
+    <x:row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A143" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3426,7 +3438,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="144" spans="1:6">
+    <x:row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A144" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3446,7 +3458,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="145" spans="1:6">
+    <x:row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A145" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3466,7 +3478,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="146" spans="1:6">
+    <x:row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A146" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3486,7 +3498,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="147" spans="1:6">
+    <x:row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A147" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3506,7 +3518,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="148" spans="1:6">
+    <x:row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A148" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3526,7 +3538,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="149" spans="1:6">
+    <x:row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A149" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3546,7 +3558,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="150" spans="1:6">
+    <x:row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A150" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3566,7 +3578,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="151" spans="1:6">
+    <x:row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A151" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3586,7 +3598,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="152" spans="1:6">
+    <x:row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A152" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3606,7 +3618,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="153" spans="1:6">
+    <x:row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A153" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3626,7 +3638,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="154" spans="1:6">
+    <x:row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A154" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3646,7 +3658,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="155" spans="1:6">
+    <x:row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A155" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -3666,7 +3678,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="156" spans="1:6">
+    <x:row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A156" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3686,7 +3698,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="157" spans="1:6">
+    <x:row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A157" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3706,7 +3718,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="158" spans="1:6">
+    <x:row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A158" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3726,7 +3738,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="159" spans="1:6">
+    <x:row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A159" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3746,7 +3758,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="160" spans="1:6">
+    <x:row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A160" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3766,7 +3778,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="161" spans="1:6">
+    <x:row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A161" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3786,7 +3798,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="162" spans="1:6">
+    <x:row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A162" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3806,7 +3818,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="163" spans="1:6">
+    <x:row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A163" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3826,7 +3838,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="164" spans="1:6">
+    <x:row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A164" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3846,7 +3858,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="165" spans="1:6">
+    <x:row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A165" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -3864,11 +3876,31 @@
       </x:c>
       <x:c r="F165" s="0">
         <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <x:c r="A166" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B166" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C166" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D166" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="E166" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F166" s="0">
+        <x:v>12225</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed user interface logics
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -97,25 +97,25 @@
     <x:t>Hliran2@</x:t>
   </x:si>
   <x:si>
+    <x:t>udiel123</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bro</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>m@g.c</x:t>
+  </x:si>
+  <x:si>
     <x:t>moses</x:t>
   </x:si>
   <x:si>
-    <x:t>bro</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>m@g.c</x:t>
-  </x:si>
-  <x:si>
     <x:t>udi</x:t>
   </x:si>
   <x:si>
     <x:t>udi@udi</x:t>
-  </x:si>
-  <x:si>
-    <x:t>udiel123</x:t>
   </x:si>
   <x:si>
     <x:t>1234567</x:t>
@@ -700,7 +700,7 @@
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A7" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>21</x:v>
@@ -720,7 +720,7 @@
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A8" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>21</x:v>
@@ -740,7 +740,7 @@
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A9" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>21</x:v>
@@ -760,7 +760,7 @@
     </x:row>
     <x:row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A10" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>21</x:v>
@@ -780,7 +780,7 @@
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A11" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>21</x:v>
@@ -800,7 +800,7 @@
     </x:row>
     <x:row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A12" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>21</x:v>
@@ -820,7 +820,7 @@
     </x:row>
     <x:row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A13" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>21</x:v>
@@ -840,7 +840,7 @@
     </x:row>
     <x:row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A14" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>21</x:v>
@@ -860,7 +860,7 @@
     </x:row>
     <x:row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A15" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
         <x:v>21</x:v>
@@ -880,7 +880,7 @@
     </x:row>
     <x:row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A16" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>21</x:v>
@@ -900,7 +900,7 @@
     </x:row>
     <x:row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A17" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
         <x:v>21</x:v>
@@ -920,7 +920,7 @@
     </x:row>
     <x:row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A18" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>21</x:v>
@@ -940,7 +940,7 @@
     </x:row>
     <x:row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A19" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
         <x:v>21</x:v>
@@ -960,7 +960,7 @@
     </x:row>
     <x:row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A20" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
         <x:v>21</x:v>
@@ -980,7 +980,7 @@
     </x:row>
     <x:row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A21" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
         <x:v>21</x:v>
@@ -1000,7 +1000,7 @@
     </x:row>
     <x:row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A22" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B22" s="0" t="s">
         <x:v>21</x:v>
@@ -1020,7 +1020,7 @@
     </x:row>
     <x:row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A23" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B23" s="0" t="s">
         <x:v>21</x:v>
@@ -1040,7 +1040,7 @@
     </x:row>
     <x:row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A24" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
         <x:v>21</x:v>
@@ -1060,7 +1060,7 @@
     </x:row>
     <x:row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A25" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
         <x:v>21</x:v>
@@ -1080,7 +1080,7 @@
     </x:row>
     <x:row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A26" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B26" s="0" t="s">
         <x:v>21</x:v>
@@ -1100,7 +1100,7 @@
     </x:row>
     <x:row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A27" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B27" s="0" t="s">
         <x:v>21</x:v>
@@ -1120,7 +1120,7 @@
     </x:row>
     <x:row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A28" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B28" s="0" t="s">
         <x:v>21</x:v>
@@ -1140,7 +1140,7 @@
     </x:row>
     <x:row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A29" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B29" s="0" t="s">
         <x:v>21</x:v>
@@ -1160,7 +1160,7 @@
     </x:row>
     <x:row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A30" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B30" s="0" t="s">
         <x:v>21</x:v>
@@ -1180,7 +1180,7 @@
     </x:row>
     <x:row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A31" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B31" s="0" t="s">
         <x:v>21</x:v>
@@ -1200,7 +1200,7 @@
     </x:row>
     <x:row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A32" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B32" s="0" t="s">
         <x:v>21</x:v>
@@ -1220,7 +1220,7 @@
     </x:row>
     <x:row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A33" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B33" s="0" t="s">
         <x:v>21</x:v>
@@ -1240,7 +1240,7 @@
     </x:row>
     <x:row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A34" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
         <x:v>21</x:v>
@@ -1260,7 +1260,7 @@
     </x:row>
     <x:row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A35" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B35" s="0" t="s">
         <x:v>21</x:v>
@@ -1280,7 +1280,7 @@
     </x:row>
     <x:row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A36" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B36" s="0" t="s">
         <x:v>21</x:v>
@@ -1300,7 +1300,7 @@
     </x:row>
     <x:row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A37" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B37" s="0" t="s">
         <x:v>21</x:v>
@@ -1320,7 +1320,7 @@
     </x:row>
     <x:row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A38" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B38" s="0" t="s">
         <x:v>21</x:v>
@@ -1340,7 +1340,7 @@
     </x:row>
     <x:row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A39" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B39" s="0" t="s">
         <x:v>21</x:v>
@@ -1360,7 +1360,7 @@
     </x:row>
     <x:row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A40" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B40" s="0" t="s">
         <x:v>21</x:v>
@@ -1380,7 +1380,7 @@
     </x:row>
     <x:row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A41" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B41" s="0" t="s">
         <x:v>21</x:v>
@@ -1400,7 +1400,7 @@
     </x:row>
     <x:row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A42" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B42" s="0" t="s">
         <x:v>21</x:v>
@@ -1420,7 +1420,7 @@
     </x:row>
     <x:row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A43" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B43" s="0" t="s">
         <x:v>21</x:v>
@@ -1440,7 +1440,7 @@
     </x:row>
     <x:row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A44" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B44" s="0" t="s">
         <x:v>21</x:v>
@@ -1460,7 +1460,7 @@
     </x:row>
     <x:row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A45" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B45" s="0" t="s">
         <x:v>21</x:v>
@@ -1480,7 +1480,7 @@
     </x:row>
     <x:row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A46" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B46" s="0" t="s">
         <x:v>21</x:v>
@@ -1500,7 +1500,7 @@
     </x:row>
     <x:row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A47" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B47" s="0" t="s">
         <x:v>21</x:v>
@@ -1520,7 +1520,7 @@
     </x:row>
     <x:row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A48" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B48" s="0" t="s">
         <x:v>21</x:v>
@@ -1540,7 +1540,7 @@
     </x:row>
     <x:row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A49" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B49" s="0" t="s">
         <x:v>21</x:v>
@@ -1560,7 +1560,7 @@
     </x:row>
     <x:row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A50" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B50" s="0" t="s">
         <x:v>21</x:v>
@@ -1580,7 +1580,7 @@
     </x:row>
     <x:row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A51" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B51" s="0" t="s">
         <x:v>21</x:v>
@@ -1600,7 +1600,7 @@
     </x:row>
     <x:row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A52" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B52" s="0" t="s">
         <x:v>21</x:v>
@@ -1620,7 +1620,7 @@
     </x:row>
     <x:row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A53" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B53" s="0" t="s">
         <x:v>21</x:v>
@@ -1640,7 +1640,7 @@
     </x:row>
     <x:row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A54" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B54" s="0" t="s">
         <x:v>21</x:v>
@@ -1660,7 +1660,7 @@
     </x:row>
     <x:row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A55" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B55" s="0" t="s">
         <x:v>21</x:v>
@@ -1680,7 +1680,7 @@
     </x:row>
     <x:row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A56" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B56" s="0" t="s">
         <x:v>21</x:v>
@@ -1700,7 +1700,7 @@
     </x:row>
     <x:row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A57" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B57" s="0" t="s">
         <x:v>21</x:v>
@@ -1720,7 +1720,7 @@
     </x:row>
     <x:row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A58" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B58" s="0" t="s">
         <x:v>21</x:v>
@@ -1740,7 +1740,7 @@
     </x:row>
     <x:row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A59" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B59" s="0" t="s">
         <x:v>21</x:v>
@@ -1760,7 +1760,7 @@
     </x:row>
     <x:row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A60" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B60" s="0" t="s">
         <x:v>21</x:v>
@@ -1780,7 +1780,7 @@
     </x:row>
     <x:row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A61" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B61" s="0" t="s">
         <x:v>21</x:v>
@@ -1800,7 +1800,7 @@
     </x:row>
     <x:row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A62" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B62" s="0" t="s">
         <x:v>21</x:v>
@@ -1820,7 +1820,7 @@
     </x:row>
     <x:row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A63" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B63" s="0" t="s">
         <x:v>21</x:v>
@@ -1840,7 +1840,7 @@
     </x:row>
     <x:row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A64" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B64" s="0" t="s">
         <x:v>21</x:v>
@@ -1860,7 +1860,7 @@
     </x:row>
     <x:row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A65" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B65" s="0" t="s">
         <x:v>21</x:v>
@@ -1880,7 +1880,7 @@
     </x:row>
     <x:row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A66" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B66" s="0" t="s">
         <x:v>21</x:v>
@@ -1900,16 +1900,16 @@
     </x:row>
     <x:row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A67" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B67" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C67" s="0">
         <x:v>1234</x:v>
       </x:c>
       <x:c r="D67" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E67" s="0" t="s">
         <x:v>17</x:v>
@@ -1920,7 +1920,7 @@
     </x:row>
     <x:row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A68" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B68" s="0" t="s">
         <x:v>21</x:v>
@@ -1940,7 +1940,7 @@
     </x:row>
     <x:row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A69" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B69" s="0" t="s">
         <x:v>21</x:v>
@@ -1960,7 +1960,7 @@
     </x:row>
     <x:row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A70" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B70" s="0" t="s">
         <x:v>21</x:v>
@@ -1980,7 +1980,7 @@
     </x:row>
     <x:row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A71" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B71" s="0" t="s">
         <x:v>21</x:v>
@@ -2000,7 +2000,7 @@
     </x:row>
     <x:row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A72" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B72" s="0" t="s">
         <x:v>21</x:v>
@@ -2020,7 +2020,7 @@
     </x:row>
     <x:row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A73" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B73" s="0" t="s">
         <x:v>21</x:v>
@@ -2040,7 +2040,7 @@
     </x:row>
     <x:row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A74" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B74" s="0" t="s">
         <x:v>21</x:v>
@@ -2060,7 +2060,7 @@
     </x:row>
     <x:row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A75" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B75" s="0" t="s">
         <x:v>21</x:v>
@@ -2080,7 +2080,7 @@
     </x:row>
     <x:row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A76" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B76" s="0" t="s">
         <x:v>21</x:v>
@@ -2100,7 +2100,7 @@
     </x:row>
     <x:row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A77" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B77" s="0" t="s">
         <x:v>21</x:v>
@@ -2120,7 +2120,7 @@
     </x:row>
     <x:row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A78" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B78" s="0" t="s">
         <x:v>21</x:v>
@@ -2140,7 +2140,7 @@
     </x:row>
     <x:row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A79" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B79" s="0" t="s">
         <x:v>21</x:v>
@@ -2160,7 +2160,7 @@
     </x:row>
     <x:row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A80" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B80" s="0" t="s">
         <x:v>21</x:v>
@@ -2180,7 +2180,7 @@
     </x:row>
     <x:row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A81" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B81" s="0" t="s">
         <x:v>21</x:v>
@@ -2200,7 +2200,7 @@
     </x:row>
     <x:row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A82" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B82" s="0" t="s">
         <x:v>21</x:v>
@@ -2220,7 +2220,7 @@
     </x:row>
     <x:row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A83" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B83" s="0" t="s">
         <x:v>21</x:v>
@@ -2240,7 +2240,7 @@
     </x:row>
     <x:row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A84" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B84" s="0" t="s">
         <x:v>21</x:v>
@@ -2260,7 +2260,7 @@
     </x:row>
     <x:row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A85" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B85" s="0" t="s">
         <x:v>21</x:v>
@@ -2280,10 +2280,10 @@
     </x:row>
     <x:row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A86" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B86" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C86" s="0" t="s">
         <x:v>27</x:v>
@@ -2300,7 +2300,7 @@
     </x:row>
     <x:row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A87" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B87" s="0" t="s">
         <x:v>21</x:v>
@@ -2360,7 +2360,7 @@
     </x:row>
     <x:row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A90" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B90" s="0" t="s">
         <x:v>21</x:v>
@@ -2380,7 +2380,7 @@
     </x:row>
     <x:row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A91" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B91" s="0" t="s">
         <x:v>21</x:v>
@@ -2400,7 +2400,7 @@
     </x:row>
     <x:row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A92" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B92" s="0" t="s">
         <x:v>21</x:v>
@@ -2420,7 +2420,7 @@
     </x:row>
     <x:row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A93" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B93" s="0" t="s">
         <x:v>21</x:v>
@@ -2440,7 +2440,7 @@
     </x:row>
     <x:row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A94" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B94" s="0" t="s">
         <x:v>21</x:v>
@@ -2460,7 +2460,7 @@
     </x:row>
     <x:row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A95" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B95" s="0" t="s">
         <x:v>21</x:v>
@@ -2480,7 +2480,7 @@
     </x:row>
     <x:row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A96" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B96" s="0" t="s">
         <x:v>21</x:v>
@@ -2500,7 +2500,7 @@
     </x:row>
     <x:row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A97" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B97" s="0" t="s">
         <x:v>21</x:v>
@@ -2520,7 +2520,7 @@
     </x:row>
     <x:row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A98" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B98" s="0" t="s">
         <x:v>21</x:v>
@@ -2540,7 +2540,7 @@
     </x:row>
     <x:row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A99" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B99" s="0" t="s">
         <x:v>21</x:v>
@@ -2560,7 +2560,7 @@
     </x:row>
     <x:row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A100" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B100" s="0" t="s">
         <x:v>21</x:v>
@@ -2580,7 +2580,7 @@
     </x:row>
     <x:row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A101" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B101" s="0" t="s">
         <x:v>21</x:v>
@@ -2600,7 +2600,7 @@
     </x:row>
     <x:row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A102" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B102" s="0" t="s">
         <x:v>21</x:v>
@@ -2620,7 +2620,7 @@
     </x:row>
     <x:row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A103" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B103" s="0" t="s">
         <x:v>21</x:v>
@@ -2640,7 +2640,7 @@
     </x:row>
     <x:row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A104" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B104" s="0" t="s">
         <x:v>21</x:v>
@@ -2660,7 +2660,7 @@
     </x:row>
     <x:row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A105" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B105" s="0" t="s">
         <x:v>21</x:v>
@@ -2680,7 +2680,7 @@
     </x:row>
     <x:row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A106" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B106" s="0" t="s">
         <x:v>21</x:v>
@@ -2700,7 +2700,7 @@
     </x:row>
     <x:row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A107" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B107" s="0" t="s">
         <x:v>21</x:v>
@@ -2720,7 +2720,7 @@
     </x:row>
     <x:row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A108" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B108" s="0" t="s">
         <x:v>21</x:v>
@@ -2740,7 +2740,7 @@
     </x:row>
     <x:row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A109" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B109" s="0" t="s">
         <x:v>21</x:v>
@@ -2760,7 +2760,7 @@
     </x:row>
     <x:row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A110" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B110" s="0" t="s">
         <x:v>21</x:v>
@@ -2780,7 +2780,7 @@
     </x:row>
     <x:row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A111" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B111" s="0" t="s">
         <x:v>21</x:v>
@@ -2800,7 +2800,7 @@
     </x:row>
     <x:row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A112" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B112" s="0" t="s">
         <x:v>21</x:v>
@@ -2820,7 +2820,7 @@
     </x:row>
     <x:row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A113" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B113" s="0" t="s">
         <x:v>21</x:v>
@@ -2840,7 +2840,7 @@
     </x:row>
     <x:row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A114" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B114" s="0" t="s">
         <x:v>21</x:v>
@@ -2860,7 +2860,7 @@
     </x:row>
     <x:row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A115" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B115" s="0" t="s">
         <x:v>21</x:v>
@@ -2880,7 +2880,7 @@
     </x:row>
     <x:row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A116" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B116" s="0" t="s">
         <x:v>21</x:v>
@@ -2900,7 +2900,7 @@
     </x:row>
     <x:row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A117" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B117" s="0" t="s">
         <x:v>21</x:v>
@@ -2920,7 +2920,7 @@
     </x:row>
     <x:row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A118" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B118" s="0" t="s">
         <x:v>21</x:v>
@@ -2940,7 +2940,7 @@
     </x:row>
     <x:row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A119" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B119" s="0" t="s">
         <x:v>21</x:v>
@@ -2960,7 +2960,7 @@
     </x:row>
     <x:row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A120" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B120" s="0" t="s">
         <x:v>21</x:v>
@@ -2980,7 +2980,7 @@
     </x:row>
     <x:row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A121" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B121" s="0" t="s">
         <x:v>21</x:v>
@@ -3000,7 +3000,7 @@
     </x:row>
     <x:row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A122" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B122" s="0" t="s">
         <x:v>21</x:v>
@@ -3020,7 +3020,7 @@
     </x:row>
     <x:row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A123" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B123" s="0" t="s">
         <x:v>21</x:v>
@@ -3040,7 +3040,7 @@
     </x:row>
     <x:row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A124" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B124" s="0" t="s">
         <x:v>21</x:v>
@@ -3060,7 +3060,7 @@
     </x:row>
     <x:row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A125" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B125" s="0" t="s">
         <x:v>21</x:v>
@@ -3080,7 +3080,7 @@
     </x:row>
     <x:row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A126" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B126" s="0" t="s">
         <x:v>21</x:v>
@@ -3100,7 +3100,7 @@
     </x:row>
     <x:row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A127" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B127" s="0" t="s">
         <x:v>21</x:v>
@@ -3120,7 +3120,7 @@
     </x:row>
     <x:row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A128" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B128" s="0" t="s">
         <x:v>21</x:v>
@@ -3140,7 +3140,7 @@
     </x:row>
     <x:row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A129" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B129" s="0" t="s">
         <x:v>21</x:v>
@@ -3160,7 +3160,7 @@
     </x:row>
     <x:row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A130" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B130" s="0" t="s">
         <x:v>21</x:v>
@@ -3180,7 +3180,7 @@
     </x:row>
     <x:row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A131" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B131" s="0" t="s">
         <x:v>21</x:v>
@@ -3200,7 +3200,7 @@
     </x:row>
     <x:row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A132" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B132" s="0" t="s">
         <x:v>21</x:v>
@@ -3220,7 +3220,7 @@
     </x:row>
     <x:row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A133" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B133" s="0" t="s">
         <x:v>21</x:v>
@@ -3240,7 +3240,7 @@
     </x:row>
     <x:row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A134" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B134" s="0" t="s">
         <x:v>21</x:v>
@@ -3260,7 +3260,7 @@
     </x:row>
     <x:row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A135" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B135" s="0" t="s">
         <x:v>21</x:v>
@@ -3280,7 +3280,7 @@
     </x:row>
     <x:row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A136" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B136" s="0" t="s">
         <x:v>21</x:v>
@@ -3300,7 +3300,7 @@
     </x:row>
     <x:row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A137" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B137" s="0" t="s">
         <x:v>21</x:v>
@@ -3320,7 +3320,7 @@
     </x:row>
     <x:row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A138" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B138" s="0" t="s">
         <x:v>21</x:v>
@@ -3340,7 +3340,7 @@
     </x:row>
     <x:row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A139" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B139" s="0" t="s">
         <x:v>21</x:v>
@@ -3360,7 +3360,7 @@
     </x:row>
     <x:row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A140" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B140" s="0" t="s">
         <x:v>21</x:v>
@@ -3380,7 +3380,7 @@
     </x:row>
     <x:row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A141" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B141" s="0" t="s">
         <x:v>21</x:v>
@@ -3400,7 +3400,7 @@
     </x:row>
     <x:row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A142" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B142" s="0" t="s">
         <x:v>21</x:v>
@@ -3420,7 +3420,7 @@
     </x:row>
     <x:row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A143" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B143" s="0" t="s">
         <x:v>21</x:v>
@@ -3440,7 +3440,7 @@
     </x:row>
     <x:row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A144" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B144" s="0" t="s">
         <x:v>21</x:v>
@@ -3460,7 +3460,7 @@
     </x:row>
     <x:row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A145" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B145" s="0" t="s">
         <x:v>21</x:v>
@@ -3480,7 +3480,7 @@
     </x:row>
     <x:row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A146" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B146" s="0" t="s">
         <x:v>21</x:v>
@@ -3500,7 +3500,7 @@
     </x:row>
     <x:row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A147" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B147" s="0" t="s">
         <x:v>21</x:v>
@@ -3520,7 +3520,7 @@
     </x:row>
     <x:row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A148" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B148" s="0" t="s">
         <x:v>21</x:v>
@@ -3540,7 +3540,7 @@
     </x:row>
     <x:row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A149" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B149" s="0" t="s">
         <x:v>21</x:v>
@@ -3560,7 +3560,7 @@
     </x:row>
     <x:row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A150" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B150" s="0" t="s">
         <x:v>21</x:v>
@@ -3580,7 +3580,7 @@
     </x:row>
     <x:row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A151" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B151" s="0" t="s">
         <x:v>21</x:v>
@@ -3600,7 +3600,7 @@
     </x:row>
     <x:row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A152" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B152" s="0" t="s">
         <x:v>21</x:v>
@@ -3620,7 +3620,7 @@
     </x:row>
     <x:row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A153" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B153" s="0" t="s">
         <x:v>21</x:v>
@@ -3640,7 +3640,7 @@
     </x:row>
     <x:row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A154" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B154" s="0" t="s">
         <x:v>21</x:v>
@@ -3680,7 +3680,7 @@
     </x:row>
     <x:row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A156" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B156" s="0" t="s">
         <x:v>21</x:v>
@@ -3700,7 +3700,7 @@
     </x:row>
     <x:row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A157" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B157" s="0" t="s">
         <x:v>21</x:v>
@@ -3720,7 +3720,7 @@
     </x:row>
     <x:row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A158" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B158" s="0" t="s">
         <x:v>21</x:v>
@@ -3740,7 +3740,7 @@
     </x:row>
     <x:row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A159" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B159" s="0" t="s">
         <x:v>21</x:v>
@@ -3760,7 +3760,7 @@
     </x:row>
     <x:row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A160" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B160" s="0" t="s">
         <x:v>21</x:v>
@@ -3780,7 +3780,7 @@
     </x:row>
     <x:row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A161" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B161" s="0" t="s">
         <x:v>21</x:v>
@@ -3800,7 +3800,7 @@
     </x:row>
     <x:row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A162" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B162" s="0" t="s">
         <x:v>21</x:v>
@@ -3820,7 +3820,7 @@
     </x:row>
     <x:row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A163" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B163" s="0" t="s">
         <x:v>21</x:v>
@@ -3840,7 +3840,7 @@
     </x:row>
     <x:row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A164" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B164" s="0" t="s">
         <x:v>21</x:v>
@@ -3860,7 +3860,7 @@
     </x:row>
     <x:row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <x:c r="A165" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B165" s="0" t="s">
         <x:v>21</x:v>

</xml_diff>

<commit_message>
disabled maximize window in : menu' udi's game, login and register
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -3895,12 +3895,12 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F166" s="0">
-        <x:v>12225</x:v>
+        <x:v>12235</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId6"/>
+    <x:hyperlink ref="D67" r:id="rId7"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
trying implement etai's pics
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>401</x:v>
+        <x:v>504</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add condition for Etai's game
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>504</x:v>
+        <x:v>609</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId6"/>
+    <x:hyperlink ref="D67" r:id="rId7"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing etai's pics and work (didnt do what he need to do)
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>609</x:v>
+        <x:v>951</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated ilan's game data update from excel
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId6"/>
+    <x:hyperlink ref="D67" r:id="rId7"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed ilan's game showing menu when closed
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>78</x:v>
+        <x:v>115</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3900,7 +3900,7 @@
     </x:row>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="D67" r:id="rId7"/>
+    <x:hyperlink ref="D67" r:id="rId6"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished economy -> merge to master
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -695,7 +695,7 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="F6" s="0">
-        <x:v>449</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3895,7 +3895,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F166" s="0">
-        <x:v>12235</x:v>
+        <x:v>11145</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>